<commit_message>
csv file v2.0 - new attacks added
</commit_message>
<xml_diff>
--- a/knowledge-engineering/src/main/java/com/data/data.xlsx
+++ b/knowledge-engineering/src/main/java/com/data/data.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Fax\cetvrta godina\drugi semestar\inzinjering znanja\IZ_Project\knowledge-engineering\src\main\java\com\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6159F8D-D899-4410-8490-2956E871CE23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="153">
   <si>
     <t>company_name</t>
   </si>
@@ -370,17 +376,125 @@
   </si>
   <si>
     <t>[confidentiality:read_data;authirization:gain_privileges;integrity:modify_data]</t>
+  </si>
+  <si>
+    <t>alibaba</t>
+  </si>
+  <si>
+    <t>bmw</t>
+  </si>
+  <si>
+    <t>audi</t>
+  </si>
+  <si>
+    <t>porshe</t>
+  </si>
+  <si>
+    <t>volkswagen</t>
+  </si>
+  <si>
+    <t>toyota</t>
+  </si>
+  <si>
+    <t>hyundai</t>
+  </si>
+  <si>
+    <t>daimler</t>
+  </si>
+  <si>
+    <t>ford</t>
+  </si>
+  <si>
+    <t>verizon</t>
+  </si>
+  <si>
+    <t>ximedes</t>
+  </si>
+  <si>
+    <t>symphony</t>
+  </si>
+  <si>
+    <t>pretexting-via-tech-support</t>
+  </si>
+  <si>
+    <t>pretexting-via-delivery-person</t>
+  </si>
+  <si>
+    <t>pretexting-via-phone</t>
+  </si>
+  <si>
+    <t>influence-perception-of-reciprocation</t>
+  </si>
+  <si>
+    <t>influence-perception-of-scarcity</t>
+  </si>
+  <si>
+    <t>influence-perception-of-authority</t>
+  </si>
+  <si>
+    <t>influence-perception-of-liking</t>
+  </si>
+  <si>
+    <t>influence-perception-of-consensus-or-social-proof</t>
+  </si>
+  <si>
+    <t>target-influence-via-framing</t>
+  </si>
+  <si>
+    <t>influence-via-modes-of-thinking</t>
+  </si>
+  <si>
+    <t>target-influence-via-interview-and-interrogation</t>
+  </si>
+  <si>
+    <t>exor</t>
+  </si>
+  <si>
+    <t>mitsubishi</t>
+  </si>
+  <si>
+    <t>[pretexting-via-tech-support, [suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-email,suspicious-conversation-visit,pop-up-windows,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[pretexting-via-tech-support, [suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-email,suspicious-conversation-visit,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[pretexting-via-tech-support, [suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-emai,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-visit]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,suspicious-conversation-visit]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,suspicious-conversation-phone-message,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-email,ad-click,pop-up-windows,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-email,suspicious-conversation-visit,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-visit,credentials-theft]</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-email,ad-click,pop-up-windows]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,36 +853,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="119.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
-    <col min="9" max="9" width="56.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="205" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.28515625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +920,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -844,7 +958,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -882,7 +996,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -920,7 +1034,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -958,7 +1072,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -996,7 +1110,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1148,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1072,7 +1186,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1110,7 +1224,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1148,7 +1262,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1186,7 +1300,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1224,7 +1338,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1262,7 +1376,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1300,7 +1414,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1452,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1376,7 +1490,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1414,7 +1528,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1452,7 +1566,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1490,7 +1604,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1528,7 +1642,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1566,7 +1680,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1604,7 +1718,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1642,7 +1756,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1680,7 +1794,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1718,7 +1832,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1756,7 +1870,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1794,7 +1908,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1832,7 +1946,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1870,7 +1984,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1908,7 +2022,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1946,7 +2060,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -1984,7 +2098,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -2022,7 +2136,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2060,7 +2174,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2098,7 +2212,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2136,7 +2250,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2174,7 +2288,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -2212,7 +2326,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2228,6 +2342,9 @@
       <c r="E39" s="6">
         <v>52000</v>
       </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
       <c r="G39" t="s">
         <v>25</v>
       </c>
@@ -2247,7 +2364,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -2285,7 +2402,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2301,6 +2418,9 @@
       <c r="E41" s="6">
         <v>49000</v>
       </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
       <c r="G41" t="s">
         <v>25</v>
       </c>
@@ -2320,7 +2440,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2358,7 +2478,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2396,7 +2516,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2434,7 +2554,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2472,7 +2592,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2510,7 +2630,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2548,7 +2668,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -2586,7 +2706,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -2624,7 +2744,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2662,7 +2782,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2700,7 +2820,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -2738,7 +2858,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -2776,11 +2896,1259 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
-      <c r="B54" s="5"/>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="B55" s="5"/>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" s="5">
+        <v>38557</v>
+      </c>
+      <c r="C54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="6">
+        <v>107</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" t="s">
+        <v>18</v>
+      </c>
+      <c r="H54" t="s">
+        <v>95</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J54" t="s">
+        <v>107</v>
+      </c>
+      <c r="K54" t="s">
+        <v>92</v>
+      </c>
+      <c r="L54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="5">
+        <v>38778</v>
+      </c>
+      <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="6">
+        <v>100</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" t="s">
+        <v>95</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J55" t="s">
+        <v>107</v>
+      </c>
+      <c r="K55" t="s">
+        <v>92</v>
+      </c>
+      <c r="L55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" s="4">
+        <v>38851</v>
+      </c>
+      <c r="C56" t="s">
+        <v>129</v>
+      </c>
+      <c r="D56" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" s="6">
+        <v>110</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" t="s">
+        <v>95</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J56" t="s">
+        <v>107</v>
+      </c>
+      <c r="K56" t="s">
+        <v>92</v>
+      </c>
+      <c r="L56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" s="4">
+        <v>39101</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+      <c r="D57" t="s">
+        <v>145</v>
+      </c>
+      <c r="E57" s="6">
+        <v>250</v>
+      </c>
+      <c r="F57" t="s">
+        <v>44</v>
+      </c>
+      <c r="G57" t="s">
+        <v>18</v>
+      </c>
+      <c r="H57" t="s">
+        <v>95</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J57" t="s">
+        <v>107</v>
+      </c>
+      <c r="K57" t="s">
+        <v>92</v>
+      </c>
+      <c r="L57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="4">
+        <v>39166</v>
+      </c>
+      <c r="C58" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="6">
+        <v>320</v>
+      </c>
+      <c r="F58" t="s">
+        <v>44</v>
+      </c>
+      <c r="G58" t="s">
+        <v>18</v>
+      </c>
+      <c r="H58" t="s">
+        <v>95</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J58" t="s">
+        <v>107</v>
+      </c>
+      <c r="K58" t="s">
+        <v>92</v>
+      </c>
+      <c r="L58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" s="4">
+        <v>39318</v>
+      </c>
+      <c r="C59" t="s">
+        <v>130</v>
+      </c>
+      <c r="D59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" s="6">
+        <v>350</v>
+      </c>
+      <c r="F59" t="s">
+        <v>44</v>
+      </c>
+      <c r="G59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J59" t="s">
+        <v>107</v>
+      </c>
+      <c r="K59" t="s">
+        <v>92</v>
+      </c>
+      <c r="L59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="4">
+        <v>39473</v>
+      </c>
+      <c r="C60" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E60" s="6">
+        <v>110000</v>
+      </c>
+      <c r="F60" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" t="s">
+        <v>95</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J60" t="s">
+        <v>107</v>
+      </c>
+      <c r="K60" t="s">
+        <v>92</v>
+      </c>
+      <c r="L60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="4">
+        <v>39529</v>
+      </c>
+      <c r="C61" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" s="6">
+        <v>112000</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" t="s">
+        <v>25</v>
+      </c>
+      <c r="H61" t="s">
+        <v>95</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J61" t="s">
+        <v>107</v>
+      </c>
+      <c r="K61" t="s">
+        <v>92</v>
+      </c>
+      <c r="L61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="4">
+        <v>39538</v>
+      </c>
+      <c r="C62" t="s">
+        <v>131</v>
+      </c>
+      <c r="D62" t="s">
+        <v>147</v>
+      </c>
+      <c r="E62" s="6">
+        <v>120000</v>
+      </c>
+      <c r="F62" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" t="s">
+        <v>95</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J62" t="s">
+        <v>107</v>
+      </c>
+      <c r="K62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="4">
+        <v>40141</v>
+      </c>
+      <c r="C63" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" s="6">
+        <v>34000</v>
+      </c>
+      <c r="F63" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" t="s">
+        <v>25</v>
+      </c>
+      <c r="H63" t="s">
+        <v>95</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J63" t="s">
+        <v>110</v>
+      </c>
+      <c r="K63" t="s">
+        <v>92</v>
+      </c>
+      <c r="L63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="4">
+        <v>40154</v>
+      </c>
+      <c r="C64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64" t="s">
+        <v>149</v>
+      </c>
+      <c r="E64" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F64" t="s">
+        <v>31</v>
+      </c>
+      <c r="G64" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" t="s">
+        <v>95</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J64" t="s">
+        <v>110</v>
+      </c>
+      <c r="K64" t="s">
+        <v>92</v>
+      </c>
+      <c r="L64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" s="4">
+        <v>40598</v>
+      </c>
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" t="s">
+        <v>149</v>
+      </c>
+      <c r="E65" s="6">
+        <v>70430</v>
+      </c>
+      <c r="F65" t="s">
+        <v>66</v>
+      </c>
+      <c r="G65" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" t="s">
+        <v>95</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J65" t="s">
+        <v>110</v>
+      </c>
+      <c r="K65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="4">
+        <v>40612</v>
+      </c>
+      <c r="C66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" t="s">
+        <v>149</v>
+      </c>
+      <c r="E66" s="6">
+        <v>79200</v>
+      </c>
+      <c r="F66" t="s">
+        <v>66</v>
+      </c>
+      <c r="G66" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" t="s">
+        <v>95</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J66" t="s">
+        <v>110</v>
+      </c>
+      <c r="K66" t="s">
+        <v>90</v>
+      </c>
+      <c r="L66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="5">
+        <v>42024</v>
+      </c>
+      <c r="C67" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" t="s">
+        <v>149</v>
+      </c>
+      <c r="E67" s="6">
+        <v>21000</v>
+      </c>
+      <c r="F67" t="s">
+        <v>66</v>
+      </c>
+      <c r="G67" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" t="s">
+        <v>95</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J67" t="s">
+        <v>110</v>
+      </c>
+      <c r="K67" t="s">
+        <v>90</v>
+      </c>
+      <c r="L67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="4">
+        <v>43105</v>
+      </c>
+      <c r="C68" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" t="s">
+        <v>149</v>
+      </c>
+      <c r="E68" s="6">
+        <v>27000</v>
+      </c>
+      <c r="F68" t="s">
+        <v>66</v>
+      </c>
+      <c r="G68" t="s">
+        <v>52</v>
+      </c>
+      <c r="H68" t="s">
+        <v>95</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J68" t="s">
+        <v>110</v>
+      </c>
+      <c r="K68" t="s">
+        <v>90</v>
+      </c>
+      <c r="L68" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" s="4">
+        <v>43120</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" t="s">
+        <v>149</v>
+      </c>
+      <c r="E69" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F69" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" t="s">
+        <v>52</v>
+      </c>
+      <c r="H69" t="s">
+        <v>95</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J69" t="s">
+        <v>110</v>
+      </c>
+      <c r="K69" t="s">
+        <v>90</v>
+      </c>
+      <c r="L69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="4">
+        <v>43436</v>
+      </c>
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" t="s">
+        <v>149</v>
+      </c>
+      <c r="E70" s="6">
+        <v>312000</v>
+      </c>
+      <c r="F70" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" t="s">
+        <v>52</v>
+      </c>
+      <c r="H70" t="s">
+        <v>95</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J70" t="s">
+        <v>110</v>
+      </c>
+      <c r="K70" t="s">
+        <v>90</v>
+      </c>
+      <c r="L70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="4">
+        <v>43819</v>
+      </c>
+      <c r="C71" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" t="s">
+        <v>149</v>
+      </c>
+      <c r="E71" s="6">
+        <v>359542</v>
+      </c>
+      <c r="F71" t="s">
+        <v>19</v>
+      </c>
+      <c r="G71" t="s">
+        <v>42</v>
+      </c>
+      <c r="H71" t="s">
+        <v>95</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J71" t="s">
+        <v>110</v>
+      </c>
+      <c r="K71" t="s">
+        <v>90</v>
+      </c>
+      <c r="L71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" s="4">
+        <v>43960</v>
+      </c>
+      <c r="C72" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" t="s">
+        <v>150</v>
+      </c>
+      <c r="E72" s="6">
+        <v>360000</v>
+      </c>
+      <c r="F72" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72" t="s">
+        <v>42</v>
+      </c>
+      <c r="H72" t="s">
+        <v>95</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J72" t="s">
+        <v>110</v>
+      </c>
+      <c r="K72" t="s">
+        <v>92</v>
+      </c>
+      <c r="L72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" s="4">
+        <v>44036</v>
+      </c>
+      <c r="C73" t="s">
+        <v>135</v>
+      </c>
+      <c r="D73" t="s">
+        <v>150</v>
+      </c>
+      <c r="E73" s="6">
+        <v>104731</v>
+      </c>
+      <c r="F73" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" t="s">
+        <v>42</v>
+      </c>
+      <c r="H73" t="s">
+        <v>95</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J73" t="s">
+        <v>110</v>
+      </c>
+      <c r="K73" t="s">
+        <v>92</v>
+      </c>
+      <c r="L73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" s="4">
+        <v>43834</v>
+      </c>
+      <c r="C74" t="s">
+        <v>135</v>
+      </c>
+      <c r="D74" t="s">
+        <v>150</v>
+      </c>
+      <c r="E74" s="6">
+        <v>96000</v>
+      </c>
+      <c r="F74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" t="s">
+        <v>42</v>
+      </c>
+      <c r="H74" t="s">
+        <v>95</v>
+      </c>
+      <c r="I74" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J74" t="s">
+        <v>110</v>
+      </c>
+      <c r="K74" t="s">
+        <v>92</v>
+      </c>
+      <c r="L74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>124</v>
+      </c>
+      <c r="B75" s="5">
+        <v>43931</v>
+      </c>
+      <c r="C75" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" t="s">
+        <v>149</v>
+      </c>
+      <c r="E75" s="6">
+        <v>288481</v>
+      </c>
+      <c r="F75" t="s">
+        <v>44</v>
+      </c>
+      <c r="G75" t="s">
+        <v>25</v>
+      </c>
+      <c r="H75" t="s">
+        <v>95</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J75" t="s">
+        <v>110</v>
+      </c>
+      <c r="K75" t="s">
+        <v>95</v>
+      </c>
+      <c r="L75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" s="5">
+        <v>44318</v>
+      </c>
+      <c r="C76" t="s">
+        <v>136</v>
+      </c>
+      <c r="D76" t="s">
+        <v>149</v>
+      </c>
+      <c r="E76" s="6">
+        <v>289481</v>
+      </c>
+      <c r="F76" t="s">
+        <v>44</v>
+      </c>
+      <c r="G76" t="s">
+        <v>25</v>
+      </c>
+      <c r="H76" t="s">
+        <v>95</v>
+      </c>
+      <c r="I76" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J76" t="s">
+        <v>110</v>
+      </c>
+      <c r="K76" t="s">
+        <v>95</v>
+      </c>
+      <c r="L76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="5">
+        <v>40385</v>
+      </c>
+      <c r="C77" t="s">
+        <v>136</v>
+      </c>
+      <c r="D77" t="s">
+        <v>149</v>
+      </c>
+      <c r="E77" s="6">
+        <v>190000</v>
+      </c>
+      <c r="F77" t="s">
+        <v>31</v>
+      </c>
+      <c r="G77" t="s">
+        <v>25</v>
+      </c>
+      <c r="H77" t="s">
+        <v>95</v>
+      </c>
+      <c r="I77" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J77" t="s">
+        <v>110</v>
+      </c>
+      <c r="K77" t="s">
+        <v>95</v>
+      </c>
+      <c r="L77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>125</v>
+      </c>
+      <c r="B78" s="5">
+        <v>40557</v>
+      </c>
+      <c r="C78" t="s">
+        <v>137</v>
+      </c>
+      <c r="D78" t="s">
+        <v>149</v>
+      </c>
+      <c r="E78" s="6">
+        <v>230000</v>
+      </c>
+      <c r="F78" t="s">
+        <v>31</v>
+      </c>
+      <c r="G78" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" t="s">
+        <v>92</v>
+      </c>
+      <c r="I78" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J78" t="s">
+        <v>107</v>
+      </c>
+      <c r="K78" t="s">
+        <v>95</v>
+      </c>
+      <c r="L78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" s="5">
+        <v>40929</v>
+      </c>
+      <c r="C79" t="s">
+        <v>137</v>
+      </c>
+      <c r="D79" t="s">
+        <v>149</v>
+      </c>
+      <c r="E79" s="6">
+        <v>132200</v>
+      </c>
+      <c r="F79" t="s">
+        <v>31</v>
+      </c>
+      <c r="G79" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79" t="s">
+        <v>92</v>
+      </c>
+      <c r="I79" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J79" t="s">
+        <v>107</v>
+      </c>
+      <c r="K79" t="s">
+        <v>95</v>
+      </c>
+      <c r="L79" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="5">
+        <v>41008</v>
+      </c>
+      <c r="C80" t="s">
+        <v>137</v>
+      </c>
+      <c r="D80" t="s">
+        <v>149</v>
+      </c>
+      <c r="E80" s="6">
+        <v>132203</v>
+      </c>
+      <c r="F80" t="s">
+        <v>31</v>
+      </c>
+      <c r="G80" t="s">
+        <v>18</v>
+      </c>
+      <c r="H80" t="s">
+        <v>92</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J80" t="s">
+        <v>107</v>
+      </c>
+      <c r="K80" t="s">
+        <v>95</v>
+      </c>
+      <c r="L80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="5">
+        <v>42262</v>
+      </c>
+      <c r="C81" t="s">
+        <v>138</v>
+      </c>
+      <c r="D81" t="s">
+        <v>151</v>
+      </c>
+      <c r="E81" s="6">
+        <v>143000</v>
+      </c>
+      <c r="F81" t="s">
+        <v>31</v>
+      </c>
+      <c r="G81" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81" t="s">
+        <v>92</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J81" t="s">
+        <v>110</v>
+      </c>
+      <c r="K81" t="s">
+        <v>92</v>
+      </c>
+      <c r="L81" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" s="5">
+        <v>41791</v>
+      </c>
+      <c r="C82" t="s">
+        <v>138</v>
+      </c>
+      <c r="D82" t="s">
+        <v>151</v>
+      </c>
+      <c r="E82" s="6">
+        <v>123</v>
+      </c>
+      <c r="F82" t="s">
+        <v>66</v>
+      </c>
+      <c r="G82" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" t="s">
+        <v>92</v>
+      </c>
+      <c r="I82" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J82" t="s">
+        <v>110</v>
+      </c>
+      <c r="K82" t="s">
+        <v>92</v>
+      </c>
+      <c r="L82" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" s="5">
+        <v>41772</v>
+      </c>
+      <c r="C83" t="s">
+        <v>138</v>
+      </c>
+      <c r="D83" t="s">
+        <v>151</v>
+      </c>
+      <c r="E83" s="6">
+        <v>8</v>
+      </c>
+      <c r="F83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G83" t="s">
+        <v>16</v>
+      </c>
+      <c r="H83" t="s">
+        <v>92</v>
+      </c>
+      <c r="I83" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J83" t="s">
+        <v>110</v>
+      </c>
+      <c r="K83" t="s">
+        <v>92</v>
+      </c>
+      <c r="L83" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>141</v>
+      </c>
+      <c r="B84" s="5">
+        <v>42859</v>
+      </c>
+      <c r="C84" t="s">
+        <v>139</v>
+      </c>
+      <c r="D84" t="s">
+        <v>152</v>
+      </c>
+      <c r="E84" s="6">
+        <v>6</v>
+      </c>
+      <c r="F84" t="s">
+        <v>66</v>
+      </c>
+      <c r="G84" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" t="s">
+        <v>90</v>
+      </c>
+      <c r="I84" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J84" t="s">
+        <v>110</v>
+      </c>
+      <c r="K84" t="s">
+        <v>92</v>
+      </c>
+      <c r="L84" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>141</v>
+      </c>
+      <c r="B85" s="5">
+        <v>44012</v>
+      </c>
+      <c r="C85" t="s">
+        <v>139</v>
+      </c>
+      <c r="D85" t="s">
+        <v>152</v>
+      </c>
+      <c r="E85" s="6">
+        <v>31</v>
+      </c>
+      <c r="F85" t="s">
+        <v>66</v>
+      </c>
+      <c r="G85" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" t="s">
+        <v>90</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J85" t="s">
+        <v>110</v>
+      </c>
+      <c r="K85" t="s">
+        <v>92</v>
+      </c>
+      <c r="L85" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" s="5">
+        <v>43568</v>
+      </c>
+      <c r="C86" t="s">
+        <v>139</v>
+      </c>
+      <c r="D86" t="s">
+        <v>152</v>
+      </c>
+      <c r="E86" s="6">
+        <v>234</v>
+      </c>
+      <c r="F86" t="s">
+        <v>66</v>
+      </c>
+      <c r="G86" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" t="s">
+        <v>90</v>
+      </c>
+      <c r="I86" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J86" t="s">
+        <v>110</v>
+      </c>
+      <c r="K86" t="s">
+        <v>92</v>
+      </c>
+      <c r="L86" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
csv file v2.1 - new attacks added
</commit_message>
<xml_diff>
--- a/knowledge-engineering/src/main/java/com/data/data.xlsx
+++ b/knowledge-engineering/src/main/java/com/data/data.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Fax\cetvrta godina\drugi semestar\inzinjering znanja\IZ_Project\knowledge-engineering\src\main\java\com\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6159F8D-D899-4410-8490-2956E871CE23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="163">
   <si>
     <t>company_name</t>
   </si>
@@ -484,17 +478,47 @@
   </si>
   <si>
     <t>[suspicious-conversation-phone-call,suspicious-conversation-phone-message,suspicious-conversation-email,ad-click,pop-up-windows]</t>
+  </si>
+  <si>
+    <t>pharming</t>
+  </si>
+  <si>
+    <t>[suspicious-link,suspicious-website,credential-re-entering,credentials-theft,virus-detection]</t>
+  </si>
+  <si>
+    <t>vulnerable_DNS</t>
+  </si>
+  <si>
+    <t>voice-phishing</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-phone-call,credentials-theft,frequents-spams]</t>
+  </si>
+  <si>
+    <t>sound-squatting</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-email,suspicious-link,suspicious-website,credentials-theft,frequents-spams]</t>
+  </si>
+  <si>
+    <t>homograph-attack-via-homoglyphs</t>
+  </si>
+  <si>
+    <t>sia</t>
+  </si>
+  <si>
+    <t>bit-squatting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -853,36 +877,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:XFD86"/>
+    <sheetView tabSelected="1" topLeftCell="E64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L101" sqref="L101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="205" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="56.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="56.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.33203125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +944,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -958,7 +982,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -996,7 +1020,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1058,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1072,7 +1096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1110,7 +1134,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1172,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1186,7 +1210,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1224,7 +1248,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1262,7 +1286,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1300,7 +1324,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1338,7 +1362,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1376,7 +1400,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1414,7 +1438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1452,7 +1476,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1490,7 +1514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1528,7 +1552,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1566,7 +1590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1604,7 +1628,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1642,7 +1666,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1680,7 +1704,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1718,7 +1742,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1756,7 +1780,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1794,7 +1818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1832,7 +1856,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1870,7 +1894,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1908,7 +1932,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1946,7 +1970,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1984,7 +2008,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2022,7 +2046,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2060,7 +2084,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -2098,7 +2122,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -2136,7 +2160,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2174,7 +2198,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2212,7 +2236,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2250,7 +2274,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2288,7 +2312,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -2326,7 +2350,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2364,7 +2388,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -2402,7 +2426,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2440,7 +2464,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2478,7 +2502,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2516,7 +2540,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2554,7 +2578,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2592,7 +2616,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2630,7 +2654,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2668,7 +2692,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -2706,7 +2730,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -2744,7 +2768,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2782,7 +2806,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2820,7 +2844,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -2858,7 +2882,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -2896,7 +2920,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>127</v>
       </c>
@@ -2934,7 +2958,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -2972,7 +2996,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -3010,7 +3034,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>128</v>
       </c>
@@ -3048,7 +3072,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>128</v>
       </c>
@@ -3086,7 +3110,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>128</v>
       </c>
@@ -3124,7 +3148,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>117</v>
       </c>
@@ -3162,7 +3186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -3200,7 +3224,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -3238,7 +3262,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -3276,7 +3300,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>118</v>
       </c>
@@ -3314,7 +3338,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -3352,7 +3376,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>119</v>
       </c>
@@ -3390,7 +3414,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>120</v>
       </c>
@@ -3428,7 +3452,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>120</v>
       </c>
@@ -3466,7 +3490,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>121</v>
       </c>
@@ -3504,7 +3528,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>121</v>
       </c>
@@ -3542,7 +3566,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>122</v>
       </c>
@@ -3580,7 +3604,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>122</v>
       </c>
@@ -3618,7 +3642,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>123</v>
       </c>
@@ -3656,7 +3680,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>123</v>
       </c>
@@ -3694,7 +3718,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>124</v>
       </c>
@@ -3732,7 +3756,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>124</v>
       </c>
@@ -3770,7 +3794,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>125</v>
       </c>
@@ -3808,7 +3832,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>125</v>
       </c>
@@ -3846,7 +3870,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>126</v>
       </c>
@@ -3884,7 +3908,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>126</v>
       </c>
@@ -3922,7 +3946,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>126</v>
       </c>
@@ -3960,7 +3984,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -3998,7 +4022,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>140</v>
       </c>
@@ -4036,7 +4060,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>141</v>
       </c>
@@ -4074,7 +4098,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>141</v>
       </c>
@@ -4112,7 +4136,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>141</v>
       </c>
@@ -4148,6 +4172,567 @@
       </c>
       <c r="L86" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87" s="4">
+        <v>43593</v>
+      </c>
+      <c r="C87" t="s">
+        <v>153</v>
+      </c>
+      <c r="D87" t="s">
+        <v>154</v>
+      </c>
+      <c r="E87" s="6">
+        <v>350</v>
+      </c>
+      <c r="F87" t="s">
+        <v>19</v>
+      </c>
+      <c r="G87" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87" t="s">
+        <v>92</v>
+      </c>
+      <c r="I87" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J87" t="s">
+        <v>111</v>
+      </c>
+      <c r="K87" t="s">
+        <v>90</v>
+      </c>
+      <c r="L87" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" s="4">
+        <v>44114</v>
+      </c>
+      <c r="C88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E88" s="6">
+        <v>800</v>
+      </c>
+      <c r="F88" t="s">
+        <v>19</v>
+      </c>
+      <c r="G88" t="s">
+        <v>18</v>
+      </c>
+      <c r="H88" t="s">
+        <v>92</v>
+      </c>
+      <c r="I88" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J88" t="s">
+        <v>111</v>
+      </c>
+      <c r="K88" t="s">
+        <v>90</v>
+      </c>
+      <c r="L88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89" s="4">
+        <v>44232</v>
+      </c>
+      <c r="C89" t="s">
+        <v>153</v>
+      </c>
+      <c r="D89" t="s">
+        <v>154</v>
+      </c>
+      <c r="E89" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F89" t="s">
+        <v>8</v>
+      </c>
+      <c r="G89" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" t="s">
+        <v>92</v>
+      </c>
+      <c r="I89" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J89" t="s">
+        <v>111</v>
+      </c>
+      <c r="K89" t="s">
+        <v>90</v>
+      </c>
+      <c r="L89" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" t="s">
+        <v>60</v>
+      </c>
+      <c r="B90" s="4">
+        <v>40001</v>
+      </c>
+      <c r="C90" t="s">
+        <v>156</v>
+      </c>
+      <c r="D90" t="s">
+        <v>157</v>
+      </c>
+      <c r="E90" s="6">
+        <v>150</v>
+      </c>
+      <c r="F90" t="s">
+        <v>8</v>
+      </c>
+      <c r="G90" t="s">
+        <v>18</v>
+      </c>
+      <c r="H90" t="s">
+        <v>92</v>
+      </c>
+      <c r="I90" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J90" t="s">
+        <v>105</v>
+      </c>
+      <c r="K90" t="s">
+        <v>90</v>
+      </c>
+      <c r="L90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" t="s">
+        <v>62</v>
+      </c>
+      <c r="B91" s="4">
+        <v>41620</v>
+      </c>
+      <c r="C91" t="s">
+        <v>156</v>
+      </c>
+      <c r="D91" t="s">
+        <v>157</v>
+      </c>
+      <c r="E91" s="6">
+        <v>200000</v>
+      </c>
+      <c r="F91" t="s">
+        <v>81</v>
+      </c>
+      <c r="G91" t="s">
+        <v>16</v>
+      </c>
+      <c r="H91" t="s">
+        <v>92</v>
+      </c>
+      <c r="I91" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J91" t="s">
+        <v>105</v>
+      </c>
+      <c r="K91" t="s">
+        <v>90</v>
+      </c>
+      <c r="L91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" t="s">
+        <v>127</v>
+      </c>
+      <c r="B92" s="4">
+        <v>43592</v>
+      </c>
+      <c r="C92" t="s">
+        <v>156</v>
+      </c>
+      <c r="D92" t="s">
+        <v>157</v>
+      </c>
+      <c r="E92" s="6">
+        <v>90</v>
+      </c>
+      <c r="F92" t="s">
+        <v>8</v>
+      </c>
+      <c r="G92" t="s">
+        <v>25</v>
+      </c>
+      <c r="H92" t="s">
+        <v>92</v>
+      </c>
+      <c r="I92" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J92" t="s">
+        <v>105</v>
+      </c>
+      <c r="K92" t="s">
+        <v>90</v>
+      </c>
+      <c r="L92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" s="4">
+        <v>43163</v>
+      </c>
+      <c r="C93" t="s">
+        <v>158</v>
+      </c>
+      <c r="D93" t="s">
+        <v>159</v>
+      </c>
+      <c r="E93" s="6">
+        <v>160000</v>
+      </c>
+      <c r="F93" t="s">
+        <v>66</v>
+      </c>
+      <c r="G93" t="s">
+        <v>52</v>
+      </c>
+      <c r="H93" t="s">
+        <v>95</v>
+      </c>
+      <c r="I93" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J93" t="s">
+        <v>107</v>
+      </c>
+      <c r="K93" t="s">
+        <v>95</v>
+      </c>
+      <c r="L93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" t="s">
+        <v>120</v>
+      </c>
+      <c r="B94" s="4">
+        <v>38635</v>
+      </c>
+      <c r="C94" t="s">
+        <v>158</v>
+      </c>
+      <c r="D94" t="s">
+        <v>159</v>
+      </c>
+      <c r="E94" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F94" t="s">
+        <v>66</v>
+      </c>
+      <c r="G94" t="s">
+        <v>16</v>
+      </c>
+      <c r="H94" t="s">
+        <v>95</v>
+      </c>
+      <c r="I94" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J94" t="s">
+        <v>107</v>
+      </c>
+      <c r="K94" t="s">
+        <v>95</v>
+      </c>
+      <c r="L94" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" t="s">
+        <v>60</v>
+      </c>
+      <c r="B95" s="4">
+        <v>41132</v>
+      </c>
+      <c r="C95" t="s">
+        <v>158</v>
+      </c>
+      <c r="D95" t="s">
+        <v>159</v>
+      </c>
+      <c r="E95" s="6">
+        <v>200</v>
+      </c>
+      <c r="F95" t="s">
+        <v>8</v>
+      </c>
+      <c r="G95" t="s">
+        <v>25</v>
+      </c>
+      <c r="H95" t="s">
+        <v>95</v>
+      </c>
+      <c r="I95" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J95" t="s">
+        <v>107</v>
+      </c>
+      <c r="K95" t="s">
+        <v>95</v>
+      </c>
+      <c r="L95" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" t="s">
+        <v>141</v>
+      </c>
+      <c r="B96" s="4">
+        <v>43625</v>
+      </c>
+      <c r="C96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D96" t="s">
+        <v>159</v>
+      </c>
+      <c r="E96" s="6">
+        <v>240000</v>
+      </c>
+      <c r="F96" t="s">
+        <v>66</v>
+      </c>
+      <c r="G96" t="s">
+        <v>161</v>
+      </c>
+      <c r="H96" t="s">
+        <v>95</v>
+      </c>
+      <c r="I96" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J96" t="s">
+        <v>107</v>
+      </c>
+      <c r="K96" t="s">
+        <v>95</v>
+      </c>
+      <c r="L96" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97" t="s">
+        <v>122</v>
+      </c>
+      <c r="B97" s="4">
+        <v>44146</v>
+      </c>
+      <c r="C97" t="s">
+        <v>160</v>
+      </c>
+      <c r="D97" t="s">
+        <v>159</v>
+      </c>
+      <c r="E97" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F97" t="s">
+        <v>19</v>
+      </c>
+      <c r="G97" t="s">
+        <v>42</v>
+      </c>
+      <c r="H97" t="s">
+        <v>95</v>
+      </c>
+      <c r="I97" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J97" t="s">
+        <v>107</v>
+      </c>
+      <c r="K97" t="s">
+        <v>95</v>
+      </c>
+      <c r="L97" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" t="s">
+        <v>57</v>
+      </c>
+      <c r="B98" s="4">
+        <v>39578</v>
+      </c>
+      <c r="C98" t="s">
+        <v>160</v>
+      </c>
+      <c r="D98" t="s">
+        <v>159</v>
+      </c>
+      <c r="E98" s="6">
+        <v>400000</v>
+      </c>
+      <c r="F98" t="s">
+        <v>8</v>
+      </c>
+      <c r="G98" t="s">
+        <v>16</v>
+      </c>
+      <c r="H98" t="s">
+        <v>95</v>
+      </c>
+      <c r="I98" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J98" t="s">
+        <v>107</v>
+      </c>
+      <c r="K98" t="s">
+        <v>95</v>
+      </c>
+      <c r="L98" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="4">
+        <v>43120</v>
+      </c>
+      <c r="C99" t="s">
+        <v>162</v>
+      </c>
+      <c r="D99" t="s">
+        <v>159</v>
+      </c>
+      <c r="E99" s="6">
+        <v>100</v>
+      </c>
+      <c r="G99" t="s">
+        <v>18</v>
+      </c>
+      <c r="H99" t="s">
+        <v>95</v>
+      </c>
+      <c r="I99" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J99" t="s">
+        <v>107</v>
+      </c>
+      <c r="K99" t="s">
+        <v>95</v>
+      </c>
+      <c r="L99" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" t="s">
+        <v>60</v>
+      </c>
+      <c r="B100" s="4">
+        <v>40612</v>
+      </c>
+      <c r="C100" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" t="s">
+        <v>159</v>
+      </c>
+      <c r="E100" s="6">
+        <v>350000</v>
+      </c>
+      <c r="G100" t="s">
+        <v>25</v>
+      </c>
+      <c r="H100" t="s">
+        <v>95</v>
+      </c>
+      <c r="I100" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J100" t="s">
+        <v>107</v>
+      </c>
+      <c r="K100" t="s">
+        <v>95</v>
+      </c>
+      <c r="L100" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" t="s">
+        <v>122</v>
+      </c>
+      <c r="B101" s="4">
+        <v>43568</v>
+      </c>
+      <c r="C101" t="s">
+        <v>162</v>
+      </c>
+      <c r="D101" t="s">
+        <v>159</v>
+      </c>
+      <c r="E101" s="6">
+        <v>190000</v>
+      </c>
+      <c r="G101" t="s">
+        <v>42</v>
+      </c>
+      <c r="H101" t="s">
+        <v>95</v>
+      </c>
+      <c r="I101" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J101" t="s">
+        <v>107</v>
+      </c>
+      <c r="K101" t="s">
+        <v>95</v>
+      </c>
+      <c r="L101" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pl file v2.3 - new attacks added
</commit_message>
<xml_diff>
--- a/knowledge-engineering/src/main/java/com/data/data.xlsx
+++ b/knowledge-engineering/src/main/java/com/data/data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\inz\IZ_Project\knowledge-engineering\src\main\java\com\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="163">
   <si>
     <t>company_name</t>
   </si>
@@ -513,12 +518,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,21 +882,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L101" sqref="L101"/>
+    <sheetView tabSelected="1" topLeftCell="E88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
@@ -906,7 +911,7 @@
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +949,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -982,7 +987,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1020,7 +1025,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1058,7 +1063,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1139,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1172,7 +1177,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1210,7 +1215,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1248,7 +1253,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1286,7 +1291,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1324,7 +1329,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1362,7 +1367,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1400,7 +1405,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1438,7 +1443,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1476,7 +1481,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1552,7 +1557,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1590,7 +1595,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1628,7 +1633,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1666,7 +1671,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1704,7 +1709,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1742,7 +1747,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1780,7 +1785,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1818,7 +1823,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1856,7 +1861,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1894,7 +1899,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1932,7 +1937,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1970,7 +1975,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -2008,7 +2013,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2046,7 +2051,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2084,7 +2089,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -2160,7 +2165,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2198,7 +2203,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2236,7 +2241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2274,7 +2279,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2312,7 +2317,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -2350,7 +2355,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2388,7 +2393,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -2426,7 +2431,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2464,7 +2469,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2502,7 +2507,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2540,7 +2545,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2578,7 +2583,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2616,7 +2621,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2654,7 +2659,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2692,7 +2697,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -2768,7 +2773,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2806,7 +2811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2844,7 +2849,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -2882,7 +2887,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -2920,7 +2925,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>127</v>
       </c>
@@ -2958,7 +2963,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -2996,7 +3001,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -3034,7 +3039,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>128</v>
       </c>
@@ -3072,7 +3077,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>128</v>
       </c>
@@ -3110,7 +3115,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>128</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>117</v>
       </c>
@@ -3186,7 +3191,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -3224,7 +3229,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -3300,7 +3305,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>118</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -3376,7 +3381,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>119</v>
       </c>
@@ -3414,7 +3419,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>120</v>
       </c>
@@ -3452,7 +3457,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>120</v>
       </c>
@@ -3490,7 +3495,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>121</v>
       </c>
@@ -3528,7 +3533,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>121</v>
       </c>
@@ -3566,7 +3571,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>122</v>
       </c>
@@ -3604,7 +3609,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>122</v>
       </c>
@@ -3642,7 +3647,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>123</v>
       </c>
@@ -3680,7 +3685,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>123</v>
       </c>
@@ -3718,7 +3723,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>124</v>
       </c>
@@ -3756,7 +3761,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>124</v>
       </c>
@@ -3794,7 +3799,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>125</v>
       </c>
@@ -3832,7 +3837,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>125</v>
       </c>
@@ -3870,7 +3875,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>126</v>
       </c>
@@ -3908,7 +3913,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>126</v>
       </c>
@@ -3946,7 +3951,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>126</v>
       </c>
@@ -3984,7 +3989,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -4022,7 +4027,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>140</v>
       </c>
@@ -4060,7 +4065,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>141</v>
       </c>
@@ -4098,7 +4103,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>141</v>
       </c>
@@ -4136,7 +4141,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>141</v>
       </c>
@@ -4174,7 +4179,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -4212,7 +4217,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -4250,7 +4255,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -4288,7 +4293,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>60</v>
       </c>
@@ -4326,7 +4331,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>62</v>
       </c>
@@ -4364,7 +4369,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>127</v>
       </c>
@@ -4402,7 +4407,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>120</v>
       </c>
@@ -4440,7 +4445,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>120</v>
       </c>
@@ -4478,7 +4483,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>60</v>
       </c>
@@ -4516,7 +4521,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>141</v>
       </c>
@@ -4554,7 +4559,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>122</v>
       </c>
@@ -4592,7 +4597,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>57</v>
       </c>
@@ -4630,7 +4635,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4646,6 +4651,9 @@
       <c r="E99" s="6">
         <v>100</v>
       </c>
+      <c r="F99" t="s">
+        <v>8</v>
+      </c>
       <c r="G99" t="s">
         <v>18</v>
       </c>
@@ -4665,7 +4673,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>60</v>
       </c>
@@ -4681,6 +4689,9 @@
       <c r="E100" s="6">
         <v>350000</v>
       </c>
+      <c r="F100" t="s">
+        <v>8</v>
+      </c>
       <c r="G100" t="s">
         <v>25</v>
       </c>
@@ -4700,7 +4711,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>122</v>
       </c>
@@ -4716,6 +4727,9 @@
       <c r="E101" s="6">
         <v>190000</v>
       </c>
+      <c r="F101" t="s">
+        <v>66</v>
+      </c>
       <c r="G101" t="s">
         <v>42</v>
       </c>
@@ -4734,6 +4748,44 @@
       <c r="L101" t="s">
         <v>92</v>
       </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B102" s="4"/>
+      <c r="E102" s="6"/>
+      <c r="I102" s="11"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B103" s="4"/>
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B104" s="4"/>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B105" s="4"/>
+      <c r="E105" s="6"/>
+      <c r="I105" s="11"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B106" s="4"/>
+      <c r="E106" s="6"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B107" s="4"/>
+      <c r="E107" s="6"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B108" s="4"/>
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B109" s="4"/>
+      <c r="E109" s="6"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B110" s="4"/>
+      <c r="E110" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
csv file v2.3 - new attacks added
</commit_message>
<xml_diff>
--- a/knowledge-engineering/src/main/java/com/data/data.xlsx
+++ b/knowledge-engineering/src/main/java/com/data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="176">
   <si>
     <t>company_name</t>
   </si>
@@ -513,6 +513,45 @@
   </si>
   <si>
     <t>bit-squatting</t>
+  </si>
+  <si>
+    <t>flash-file-overlay</t>
+  </si>
+  <si>
+    <t>[suspicious-conversation-email, ad-click,suspicious-link,credentials-theft,frequents-spams]</t>
+  </si>
+  <si>
+    <t>support_invisible_flash</t>
+  </si>
+  <si>
+    <t>android-activity-hijack</t>
+  </si>
+  <si>
+    <t>tapjacking</t>
+  </si>
+  <si>
+    <t>[app-download,credentials-theft,suspicious-code-modifications]</t>
+  </si>
+  <si>
+    <t>[pop-up-windows,app-download,ad-click,frequents-spams]</t>
+  </si>
+  <si>
+    <t>previously_installed_malicious_application_on_android_device</t>
+  </si>
+  <si>
+    <t>previously_installed_malicious_application</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>rooting-sim-cards</t>
+  </si>
+  <si>
+    <t>[update,suspicious-conversation-phone-message,credentials-theft]</t>
+  </si>
+  <si>
+    <t>sim-card-that-relies-on-des-cipher</t>
   </si>
 </sst>
 </file>
@@ -890,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L110"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J100" sqref="J100"/>
+    <sheetView tabSelected="1" topLeftCell="G94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K113" sqref="K113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4750,42 +4789,460 @@
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B102" s="4"/>
-      <c r="E102" s="6"/>
-      <c r="I102" s="11"/>
+      <c r="A102" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="4">
+        <v>43444</v>
+      </c>
+      <c r="C102" t="s">
+        <v>163</v>
+      </c>
+      <c r="D102" t="s">
+        <v>164</v>
+      </c>
+      <c r="E102" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F102" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" t="s">
+        <v>16</v>
+      </c>
+      <c r="H102" t="s">
+        <v>90</v>
+      </c>
+      <c r="I102" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J102" t="s">
+        <v>105</v>
+      </c>
+      <c r="K102" t="s">
+        <v>92</v>
+      </c>
+      <c r="L102" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B103" s="4"/>
-      <c r="E103" s="6"/>
+      <c r="A103" t="s">
+        <v>117</v>
+      </c>
+      <c r="B103" s="4">
+        <v>44251</v>
+      </c>
+      <c r="C103" t="s">
+        <v>163</v>
+      </c>
+      <c r="D103" t="s">
+        <v>164</v>
+      </c>
+      <c r="E103" s="6">
+        <v>15000</v>
+      </c>
+      <c r="F103" t="s">
+        <v>8</v>
+      </c>
+      <c r="G103" t="s">
+        <v>25</v>
+      </c>
+      <c r="H103" t="s">
+        <v>90</v>
+      </c>
+      <c r="I103" t="s">
+        <v>165</v>
+      </c>
+      <c r="J103" t="s">
+        <v>105</v>
+      </c>
+      <c r="K103" t="s">
+        <v>92</v>
+      </c>
+      <c r="L103" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B104" s="4"/>
-      <c r="E104" s="6"/>
+      <c r="A104" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" s="4">
+        <v>44092</v>
+      </c>
+      <c r="C104" t="s">
+        <v>163</v>
+      </c>
+      <c r="D104" t="s">
+        <v>164</v>
+      </c>
+      <c r="E104" s="6">
+        <v>220</v>
+      </c>
+      <c r="F104" t="s">
+        <v>19</v>
+      </c>
+      <c r="G104" t="s">
+        <v>18</v>
+      </c>
+      <c r="H104" t="s">
+        <v>90</v>
+      </c>
+      <c r="I104" t="s">
+        <v>165</v>
+      </c>
+      <c r="J104" t="s">
+        <v>105</v>
+      </c>
+      <c r="K104" t="s">
+        <v>92</v>
+      </c>
+      <c r="L104" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B105" s="4"/>
-      <c r="E105" s="6"/>
-      <c r="I105" s="11"/>
+      <c r="A105" t="s">
+        <v>24</v>
+      </c>
+      <c r="B105" s="4">
+        <v>43824</v>
+      </c>
+      <c r="C105" t="s">
+        <v>166</v>
+      </c>
+      <c r="D105" t="s">
+        <v>168</v>
+      </c>
+      <c r="E105" s="6">
+        <v>1500</v>
+      </c>
+      <c r="F105" t="s">
+        <v>8</v>
+      </c>
+      <c r="G105" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105" t="s">
+        <v>90</v>
+      </c>
+      <c r="I105" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J105" t="s">
+        <v>111</v>
+      </c>
+      <c r="K105" t="s">
+        <v>92</v>
+      </c>
+      <c r="L105" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B106" s="4"/>
-      <c r="E106" s="6"/>
+      <c r="A106" t="s">
+        <v>33</v>
+      </c>
+      <c r="B106" s="4">
+        <v>44321</v>
+      </c>
+      <c r="C106" t="s">
+        <v>166</v>
+      </c>
+      <c r="D106" t="s">
+        <v>168</v>
+      </c>
+      <c r="E106" s="6">
+        <v>250</v>
+      </c>
+      <c r="F106" t="s">
+        <v>19</v>
+      </c>
+      <c r="G106" t="s">
+        <v>18</v>
+      </c>
+      <c r="H106" t="s">
+        <v>90</v>
+      </c>
+      <c r="I106" t="s">
+        <v>170</v>
+      </c>
+      <c r="J106" t="s">
+        <v>111</v>
+      </c>
+      <c r="K106" t="s">
+        <v>92</v>
+      </c>
+      <c r="L106" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B107" s="4"/>
-      <c r="E107" s="6"/>
+      <c r="A107" t="s">
+        <v>30</v>
+      </c>
+      <c r="B107" s="4">
+        <v>43936</v>
+      </c>
+      <c r="C107" t="s">
+        <v>166</v>
+      </c>
+      <c r="D107" t="s">
+        <v>168</v>
+      </c>
+      <c r="E107" s="6">
+        <v>175</v>
+      </c>
+      <c r="F107" t="s">
+        <v>19</v>
+      </c>
+      <c r="G107" t="s">
+        <v>18</v>
+      </c>
+      <c r="H107" t="s">
+        <v>90</v>
+      </c>
+      <c r="I107" t="s">
+        <v>170</v>
+      </c>
+      <c r="J107" t="s">
+        <v>111</v>
+      </c>
+      <c r="K107" t="s">
+        <v>92</v>
+      </c>
+      <c r="L107" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B108" s="4"/>
-      <c r="E108" s="6"/>
+      <c r="A108" t="s">
+        <v>17</v>
+      </c>
+      <c r="B108" s="4">
+        <v>44147</v>
+      </c>
+      <c r="C108" t="s">
+        <v>167</v>
+      </c>
+      <c r="D108" t="s">
+        <v>169</v>
+      </c>
+      <c r="E108" s="6">
+        <v>100</v>
+      </c>
+      <c r="F108" t="s">
+        <v>19</v>
+      </c>
+      <c r="G108" t="s">
+        <v>18</v>
+      </c>
+      <c r="H108" t="s">
+        <v>90</v>
+      </c>
+      <c r="I108" t="s">
+        <v>171</v>
+      </c>
+      <c r="J108" t="s">
+        <v>107</v>
+      </c>
+      <c r="K108" t="s">
+        <v>95</v>
+      </c>
+      <c r="L108" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B109" s="4"/>
-      <c r="E109" s="6"/>
+      <c r="A109" t="s">
+        <v>17</v>
+      </c>
+      <c r="B109" s="4">
+        <v>44056</v>
+      </c>
+      <c r="C109" t="s">
+        <v>167</v>
+      </c>
+      <c r="D109" t="s">
+        <v>169</v>
+      </c>
+      <c r="E109" s="6">
+        <v>100</v>
+      </c>
+      <c r="F109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G109" t="s">
+        <v>18</v>
+      </c>
+      <c r="H109" t="s">
+        <v>90</v>
+      </c>
+      <c r="I109" t="s">
+        <v>171</v>
+      </c>
+      <c r="J109" t="s">
+        <v>107</v>
+      </c>
+      <c r="K109" t="s">
+        <v>95</v>
+      </c>
+      <c r="L109" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B110" s="4"/>
-      <c r="E110" s="6"/>
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" s="4">
+        <v>43308</v>
+      </c>
+      <c r="C110" t="s">
+        <v>167</v>
+      </c>
+      <c r="D110" t="s">
+        <v>169</v>
+      </c>
+      <c r="E110" s="6">
+        <v>1500</v>
+      </c>
+      <c r="F110" t="s">
+        <v>8</v>
+      </c>
+      <c r="G110" t="s">
+        <v>25</v>
+      </c>
+      <c r="H110" t="s">
+        <v>90</v>
+      </c>
+      <c r="I110" t="s">
+        <v>171</v>
+      </c>
+      <c r="J110" t="s">
+        <v>107</v>
+      </c>
+      <c r="K110" t="s">
+        <v>95</v>
+      </c>
+      <c r="L110" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>172</v>
+      </c>
+      <c r="B111" s="4">
+        <v>43678</v>
+      </c>
+      <c r="C111" t="s">
+        <v>173</v>
+      </c>
+      <c r="D111" t="s">
+        <v>174</v>
+      </c>
+      <c r="E111" s="6">
+        <v>4200</v>
+      </c>
+      <c r="F111" t="s">
+        <v>8</v>
+      </c>
+      <c r="G111" t="s">
+        <v>16</v>
+      </c>
+      <c r="H111" t="s">
+        <v>92</v>
+      </c>
+      <c r="I111" t="s">
+        <v>175</v>
+      </c>
+      <c r="J111" t="s">
+        <v>102</v>
+      </c>
+      <c r="K111" t="s">
+        <v>90</v>
+      </c>
+      <c r="L111" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>24</v>
+      </c>
+      <c r="B112" s="4">
+        <v>43168</v>
+      </c>
+      <c r="C112" t="s">
+        <v>173</v>
+      </c>
+      <c r="D112" t="s">
+        <v>174</v>
+      </c>
+      <c r="E112" s="6">
+        <v>1500</v>
+      </c>
+      <c r="F112" t="s">
+        <v>8</v>
+      </c>
+      <c r="G112" t="s">
+        <v>25</v>
+      </c>
+      <c r="H112" t="s">
+        <v>92</v>
+      </c>
+      <c r="I112" t="s">
+        <v>175</v>
+      </c>
+      <c r="J112" t="s">
+        <v>102</v>
+      </c>
+      <c r="K112" t="s">
+        <v>90</v>
+      </c>
+      <c r="L112" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>172</v>
+      </c>
+      <c r="B113" s="4">
+        <v>44223</v>
+      </c>
+      <c r="C113" t="s">
+        <v>173</v>
+      </c>
+      <c r="D113" t="s">
+        <v>174</v>
+      </c>
+      <c r="E113" s="6">
+        <v>4200</v>
+      </c>
+      <c r="F113" t="s">
+        <v>8</v>
+      </c>
+      <c r="G113" t="s">
+        <v>16</v>
+      </c>
+      <c r="H113" t="s">
+        <v>92</v>
+      </c>
+      <c r="I113" t="s">
+        <v>175</v>
+      </c>
+      <c r="J113" t="s">
+        <v>102</v>
+      </c>
+      <c r="K113" t="s">
+        <v>90</v>
+      </c>
+      <c r="L113" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>